<commit_message>
Testing vrf determination / deploy
</commit_message>
<xml_diff>
--- a/testbed/lab_nw_auto_test.xlsx
+++ b/testbed/lab_nw_auto_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blog-videos\lab_nw_auto_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CE55D3-A327-4968-9238-F95ED2620D9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15A9490-2E86-4DD6-B25F-FA6DE04D5D5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="2295" windowWidth="21600" windowHeight="11835" xr2:uid="{F58A7B6D-CAAD-401F-8C1C-8A778D326261}"/>
+    <workbookView xWindow="-28785" yWindow="0" windowWidth="21600" windowHeight="11835" xr2:uid="{F58A7B6D-CAAD-401F-8C1C-8A778D326261}"/>
   </bookViews>
   <sheets>
     <sheet name="192.168.0.211" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
   <si>
     <t>interface</t>
   </si>
@@ -89,6 +89,36 @@
   </si>
   <si>
     <t>192.168.0.212</t>
+  </si>
+  <si>
+    <t>ospf</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>192.168.0.213</t>
+  </si>
+  <si>
+    <t>192.168.0.214</t>
+  </si>
+  <si>
+    <t>10.100.34.3</t>
+  </si>
+  <si>
+    <t>10.100.13.3</t>
+  </si>
+  <si>
+    <t>10.100.23.3</t>
+  </si>
+  <si>
+    <t>10.100.34.4</t>
+  </si>
+  <si>
+    <t>10.100.24.4</t>
+  </si>
+  <si>
+    <t>10.100.14.4</t>
   </si>
 </sst>
 </file>
@@ -440,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB7C5F9-F770-488C-AB6D-27208EF2E8E0}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +484,7 @@
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -470,8 +500,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -484,8 +517,14 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -498,8 +537,14 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -512,8 +557,14 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -526,8 +577,14 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -540,8 +597,14 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -553,6 +616,132 @@
       </c>
       <c r="D7" t="s">
         <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>